<commit_message>
Rm jdv 148 (#122)
* rm jdv 148

* update fr core 2.1.0 ccdbdcae59d9a1bad69c44e622b20435afb91d95
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-mesures-fr-observation-body-temperature.xlsx
+++ b/main/ig/StructureDefinition-mesures-fr-observation-body-temperature.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-13T15:58:46+00:00</t>
+    <t>2024-12-18T16:26:35+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -4921,7 +4921,7 @@
         <v>81</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>206</v>
+        <v>82</v>
       </c>
       <c r="AJ20" t="s" s="2">
         <v>122</v>
@@ -16224,7 +16224,7 @@
         <v>82</v>
       </c>
       <c r="X114" t="s" s="2">
-        <v>254</v>
+        <v>155</v>
       </c>
       <c r="Y114" t="s" s="2">
         <v>677</v>

</xml_diff>